<commit_message>
adjusted values for more controlled movement
</commit_message>
<xml_diff>
--- a/Robot arm/Coordinates.xlsx
+++ b/Robot arm/Coordinates.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jruoc\Documents\GitHub\Mobile-Motion-Tracking-Robot-Arm\Robot arm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff\Documents\GitHub\Mobile-Motion-Tracking-Robot-Arm\Robot arm\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6036"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="17250" windowHeight="6030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -406,14 +406,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="9.44140625" customWidth="1"/>
+    <col min="1" max="7" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -434,7 +436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -457,7 +459,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -474,13 +476,13 @@
         <v>1970</v>
       </c>
       <c r="F3" s="1">
+        <v>860</v>
+      </c>
+      <c r="G3" s="1">
         <v>1800</v>
       </c>
-      <c r="G3" s="1">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -494,10 +496,10 @@
       </c>
       <c r="F5">
         <f>SLOPE(F3:G3, F2:G2)</f>
-        <v>3133.333333333333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-3133.333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -511,13 +513,13 @@
       </c>
       <c r="F6">
         <f>INTERCEPT(F3:G3,F2:G2)</f>
-        <v>-1646.6666666666665</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4306.6666666666661</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -525,7 +527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -539,7 +541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -547,7 +549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -558,7 +560,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>0</v>
@@ -579,7 +581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -608,59 +610,59 @@
         <v>0.70000000000000007</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="1">
-        <f>B3</f>
-        <v>2500</v>
+        <f>B3-50</f>
+        <v>2450</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:G15" si="0">C3</f>
-        <v>1200</v>
+        <f>C3+50</f>
+        <v>1250</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>1080</v>
+        <f>D3-50</f>
+        <v>1030</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
-        <v>1970</v>
+        <f>E3+50</f>
+        <v>2020</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="0"/>
-        <v>1800</v>
+        <f>F3-50</f>
+        <v>810</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="0"/>
-        <v>860</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <f>G3+50</f>
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B17">
         <f>SLOPE(B15:C15, B14:C14)</f>
-        <v>1624.9999999999998</v>
+        <v>1499.9999999999998</v>
       </c>
       <c r="D17">
         <f>SLOPE(D15:E15, D14:E14)</f>
-        <v>-1112.4999999999998</v>
+        <v>-1237.4999999999998</v>
       </c>
       <c r="F17">
         <f>SLOPE(F15:G15, F14:G14)</f>
-        <v>1879.9999999999995</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-2079.9999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B18">
         <f>INTERCEPT(B15:C15,B14:C14)</f>
-        <v>1525</v>
+        <v>1550</v>
       </c>
       <c r="D18">
         <f>INTERCEPT(D15:E15,D14:E14)</f>
@@ -668,7 +670,7 @@
       </c>
       <c r="F18">
         <f>INTERCEPT(F15:G15,F14:G14)</f>
-        <v>-456</v>
+        <v>3306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>